<commit_message>
Master 2 | Varyant türkçe karakter fonksiyonu eklendi ve oluşturulan data log dosyasına kopyalandı
</commit_message>
<xml_diff>
--- a/kesim-adetleri.xlsx
+++ b/kesim-adetleri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mern-developer\planlama\kesim-adetleri-filtreleme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B4A3F0-4124-4B3D-8347-A004B22BF023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68C67B2-D205-43B7-B358-0C5A461DE413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kesim" sheetId="1" r:id="rId1"/>
@@ -213,7 +213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +229,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -288,6 +294,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -572,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,7 +827,7 @@
       <c r="C17" s="4">
         <v>936</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Master 3 | veri setine müşteri bilgisi eklendi
</commit_message>
<xml_diff>
--- a/kesim-adetleri.xlsx
+++ b/kesim-adetleri.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mern-developer\planlama\kesim-adetleri-filtreleme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68C67B2-D205-43B7-B358-0C5A461DE413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB0759B-705B-46E1-9FBA-2CE6C6B63293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kesim" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="59">
   <si>
     <t xml:space="preserve">Model </t>
   </si>
@@ -184,6 +195,24 @@
   </si>
   <si>
     <t>S53641</t>
+  </si>
+  <si>
+    <t>MÜŞTERİ</t>
+  </si>
+  <si>
+    <t>HAKRO</t>
+  </si>
+  <si>
+    <t>COMFYBALLS</t>
+  </si>
+  <si>
+    <t>SOCIEDAD</t>
+  </si>
+  <si>
+    <t>RALPH LAUREN</t>
+  </si>
+  <si>
+    <t>SELECTED FEMME</t>
   </si>
 </sst>
 </file>
@@ -239,7 +268,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -275,11 +304,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -297,6 +335,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -579,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,9 +632,10 @@
     <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,8 +648,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E1" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>281</v>
       </c>
@@ -620,8 +665,11 @@
       <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>281</v>
       </c>
@@ -634,8 +682,11 @@
       <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -648,8 +699,11 @@
       <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -662,8 +716,11 @@
       <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -676,8 +733,11 @@
       <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -690,8 +750,11 @@
       <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -704,8 +767,11 @@
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -718,8 +784,11 @@
       <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -732,8 +801,11 @@
       <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -746,8 +818,11 @@
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -760,8 +835,11 @@
       <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -774,8 +852,11 @@
       <c r="D13" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
@@ -788,8 +869,11 @@
       <c r="D14" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>281</v>
       </c>
@@ -802,8 +886,11 @@
       <c r="D15" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
@@ -816,8 +903,11 @@
       <c r="D16" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -830,8 +920,11 @@
       <c r="D17" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -844,8 +937,11 @@
       <c r="D18" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -858,8 +954,11 @@
       <c r="D19" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>471</v>
       </c>
@@ -872,8 +971,11 @@
       <c r="D20" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>471</v>
       </c>
@@ -886,8 +988,11 @@
       <c r="D21" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>816</v>
       </c>
@@ -900,8 +1005,11 @@
       <c r="D22" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>816</v>
       </c>
@@ -914,8 +1022,11 @@
       <c r="D23" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -928,8 +1039,11 @@
       <c r="D24" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>475</v>
       </c>
@@ -942,8 +1056,11 @@
       <c r="D25" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
@@ -956,8 +1073,11 @@
       <c r="D26" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>471</v>
       </c>
@@ -970,8 +1090,11 @@
       <c r="D27" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>20</v>
       </c>
@@ -984,8 +1107,11 @@
       <c r="D28" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -998,8 +1124,11 @@
       <c r="D29" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -1012,8 +1141,11 @@
       <c r="D30" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>203</v>
       </c>
@@ -1026,8 +1158,11 @@
       <c r="D31" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
@@ -1040,8 +1175,11 @@
       <c r="D32" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
@@ -1054,8 +1192,11 @@
       <c r="D33" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -1068,8 +1209,11 @@
       <c r="D34" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>5726</v>
       </c>
@@ -1082,8 +1226,11 @@
       <c r="D35" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>471</v>
       </c>
@@ -1096,8 +1243,11 @@
       <c r="D36" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>471</v>
       </c>
@@ -1110,8 +1260,11 @@
       <c r="D37" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>816</v>
       </c>
@@ -1124,8 +1277,11 @@
       <c r="D38" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>816</v>
       </c>
@@ -1138,8 +1294,11 @@
       <c r="D39" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>260</v>
       </c>
@@ -1152,8 +1311,11 @@
       <c r="D40" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
@@ -1166,8 +1328,11 @@
       <c r="D41" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>20</v>
       </c>
@@ -1180,8 +1345,11 @@
       <c r="D42" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>20</v>
       </c>
@@ -1194,8 +1362,11 @@
       <c r="D43" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>203</v>
       </c>
@@ -1208,8 +1379,11 @@
       <c r="D44" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>471</v>
       </c>
@@ -1222,8 +1396,11 @@
       <c r="D45" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>816</v>
       </c>
@@ -1235,6 +1412,9 @@
       </c>
       <c r="D46" s="5" t="s">
         <v>46</v>
+      </c>
+      <c r="E46" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>